<commit_message>
Completed validation part of email and roles
</commit_message>
<xml_diff>
--- a/uploads/Template_with_data.xlsx
+++ b/uploads/Template_with_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbjin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0866BA18-DAC0-41FF-9DA8-E67AD59C0DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D314496-4555-49AD-BA7A-7AE341391F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>First Name</t>
   </si>
@@ -57,9 +57,6 @@
     <t>adam@yourmail.com</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
     <t>Ram</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>Kazhakuttom</t>
+  </si>
+  <si>
+    <t>Student</t>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,30 +454,34 @@
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2">
+        <v>4512457889</v>
+      </c>
       <c r="F2" s="4">
         <v>33101</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="E3" s="2">
         <v>4512457889</v>
@@ -486,7 +490,7 @@
         <v>33397</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated plain template and data download
</commit_message>
<xml_diff>
--- a/uploads/Template_with_data.xlsx
+++ b/uploads/Template_with_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbjin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D314496-4555-49AD-BA7A-7AE341391F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8F7127-B468-45FF-B72C-ABE3FD0EACFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>First Name</t>
   </si>
@@ -73,6 +73,45 @@
   </si>
   <si>
     <t>Student</t>
+  </si>
+  <si>
+    <t>Jino</t>
+  </si>
+  <si>
+    <t>Mukesh</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Dhas</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>john@gmail.com</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>Jaiden</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>Marthandam</t>
+  </si>
+  <si>
+    <t>jai@yourdomain.com</t>
+  </si>
+  <si>
+    <t>Cleaner</t>
+  </si>
+  <si>
+    <t>mukesh@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -415,7 +454,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,31 +533,73 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="2">
+        <v>9876543210</v>
+      </c>
+      <c r="F4" s="4">
+        <v>32724</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2">
+        <v>784596520</v>
+      </c>
+      <c r="F5" s="4">
+        <v>32697</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="2">
+        <v>7845129630</v>
+      </c>
+      <c r="F6" s="4">
+        <v>42590</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
@@ -704,8 +785,11 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{A622EDC6-A2AE-4F39-A5EE-E6742B3FCA02}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{7AD575FC-D9BA-4F20-B3FD-106C9AD3E42A}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{B4398E00-662B-45FF-9BF0-F0330C058A9E}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{6AEE3D9A-4284-4E61-B410-0737BA598523}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{400EFE7C-0AE9-4A2F-B45D-D3F51828043E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>